<commit_message>
Re updated profit calculator
With 4th calculator explaniation
</commit_message>
<xml_diff>
--- a/HYT Calculator+Comercios.xlsx
+++ b/HYT Calculator+Comercios.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naosg\OneDrive\Escritorio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IT\Downloads\Product Manager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A109AAB9-926C-44DC-BFDC-32610F899EE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{286B4184-9F2D-4E09-ACC5-6BF5A0C6FBFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="3" xr2:uid="{0051E362-2BA8-47B0-8666-BB7F2D17AC29}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{0051E362-2BA8-47B0-8666-BB7F2D17AC29}"/>
   </bookViews>
   <sheets>
     <sheet name="Calculadora Referidos" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="71">
   <si>
     <t>Si Tienes</t>
   </si>
@@ -246,6 +246,36 @@
   <si>
     <t>USD cada una</t>
   </si>
+  <si>
+    <t>Input1, Type: Number</t>
+  </si>
+  <si>
+    <t>Input2, Type: Number</t>
+  </si>
+  <si>
+    <t>Result1, Type: Float - Input2*30</t>
+  </si>
+  <si>
+    <t>Result2, Type: Float - Input1/Result1</t>
+  </si>
+  <si>
+    <t>Result3, Type: Float, Input1*Input3</t>
+  </si>
+  <si>
+    <t>Result4, Type: Float - Input1*FixedData1</t>
+  </si>
+  <si>
+    <t>Result5, Type: Float - Result3-Result4</t>
+  </si>
+  <si>
+    <t>Result6, Type: Float (percent) - Result5/Result3</t>
+  </si>
+  <si>
+    <t>FixedData1, Type: Float (percent)</t>
+  </si>
+  <si>
+    <t>Input3, Type: Float (percent)</t>
+  </si>
 </sst>
 </file>
 
@@ -256,7 +286,7 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-&quot;$&quot;\ * #,##0_-;\-&quot;$&quot;\ * #,##0_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;\ #,##0"/>
-    <numFmt numFmtId="168" formatCode="&quot;$&quot;\ #,##0.00"/>
+    <numFmt numFmtId="166" formatCode="&quot;$&quot;\ #,##0.00"/>
   </numFmts>
   <fonts count="25" x14ac:knownFonts="1">
     <font>
@@ -449,7 +479,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -714,6 +744,21 @@
         <color indexed="64"/>
       </right>
       <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
@@ -728,7 +773,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -898,6 +943,16 @@
     <xf numFmtId="9" fontId="23" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -994,15 +1049,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -2516,9 +2567,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1851429</xdr:colOff>
+      <xdr:colOff>1854604</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>219075</xdr:rowOff>
+      <xdr:rowOff>215900</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2566,6 +2617,536 @@
         </a:extLst>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>2152650</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1219200</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Conector recto de flecha 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1B167682-FB97-47C7-979C-7491EDA905F4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="7086600" y="1524000"/>
+          <a:ext cx="2962275" cy="190500"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>2159000</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1209675</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="6" name="Conector recto de flecha 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{28E22FB7-9691-426F-967F-9F1F5378E05D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="7092950" y="1733550"/>
+          <a:ext cx="2946400" cy="190500"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>2171700</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1219200</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="Conector recto de flecha 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B1612640-E969-46F9-ABDB-5E8570993343}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="7105650" y="1914525"/>
+          <a:ext cx="2943225" cy="158750"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>2181225</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1219200</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="12" name="Conector recto de flecha 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B1612640-E969-46F9-ABDB-5E8570993343}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="7115175" y="2076450"/>
+          <a:ext cx="2933700" cy="200025"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>2228850</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="18" name="Conector recto de flecha 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{07805965-8C94-4F8E-8452-22EF9322A195}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="7162800" y="2628900"/>
+          <a:ext cx="2905125" cy="209550"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1206500</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>92075</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="21" name="Conector recto de flecha 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FDDE7165-EF40-47F6-8092-B64DC03787FF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="8531225" y="2844800"/>
+          <a:ext cx="1527175" cy="3175"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="23" name="Conector recto de flecha 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{59DE2913-0328-41CC-9637-068AF46626A5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2952750" y="3038475"/>
+          <a:ext cx="2771775" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1209675</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="29" name="Conector recto de flecha 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9F4872B2-DB0F-44C6-BD43-451B9862098D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="8839200" y="3025775"/>
+          <a:ext cx="1524000" cy="3175"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>2130425</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="30" name="Conector recto de flecha 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C56D334-43D2-4A25-8679-488E807D8A70}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="7369175" y="3486150"/>
+          <a:ext cx="2994025" cy="9525"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>2133600</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1206500</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="33" name="Conector recto de flecha 32">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DC20B2F7-30D9-413E-A19C-058FC43FF483}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="7372350" y="3752850"/>
+          <a:ext cx="2968625" cy="9525"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -2874,47 +3455,47 @@
       <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="14.5" zeroHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" customWidth="1"/>
-    <col min="2" max="2" width="22.7109375" customWidth="1"/>
-    <col min="3" max="3" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.28515625" customWidth="1"/>
-    <col min="5" max="5" width="44.140625" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" customWidth="1"/>
-    <col min="7" max="7" width="20.42578125" customWidth="1"/>
+    <col min="1" max="1" width="11.453125" customWidth="1"/>
+    <col min="2" max="2" width="22.7265625" customWidth="1"/>
+    <col min="3" max="3" width="29.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.26953125" customWidth="1"/>
+    <col min="5" max="5" width="44.1796875" customWidth="1"/>
+    <col min="6" max="6" width="11.453125" customWidth="1"/>
+    <col min="7" max="7" width="20.453125" customWidth="1"/>
     <col min="8" max="9" width="0" hidden="1" customWidth="1"/>
-    <col min="10" max="16384" width="11.42578125" hidden="1"/>
+    <col min="10" max="16384" width="11.453125" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="3" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="63"/>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-    </row>
-    <row r="2" spans="1:8" s="3" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="63"/>
-      <c r="B2" s="63"/>
-      <c r="C2" s="63"/>
-      <c r="D2" s="63"/>
-      <c r="E2" s="63"/>
-      <c r="F2" s="63"/>
-      <c r="G2" s="63"/>
-    </row>
-    <row r="3" spans="1:8" s="3" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="63"/>
-      <c r="B3" s="63"/>
-      <c r="C3" s="63"/>
-      <c r="D3" s="63"/>
-      <c r="E3" s="63"/>
-      <c r="F3" s="63"/>
-      <c r="G3" s="63"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="3" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="66"/>
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
+    </row>
+    <row r="2" spans="1:8" s="3" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="66"/>
+      <c r="B2" s="66"/>
+      <c r="C2" s="66"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="66"/>
+    </row>
+    <row r="3" spans="1:8" s="3" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="66"/>
+      <c r="B3" s="66"/>
+      <c r="C3" s="66"/>
+      <c r="D3" s="66"/>
+      <c r="E3" s="66"/>
+      <c r="F3" s="66"/>
+      <c r="G3" s="66"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="5"/>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
@@ -2923,7 +3504,7 @@
       <c r="F4" s="6"/>
       <c r="G4" s="12"/>
     </row>
-    <row r="5" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="5"/>
       <c r="B5" s="6"/>
       <c r="C5" s="21" t="s">
@@ -2938,7 +3519,7 @@
       <c r="F5" s="6"/>
       <c r="G5" s="7"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="5"/>
       <c r="B6" s="6"/>
       <c r="C6" s="8"/>
@@ -2947,7 +3528,7 @@
       <c r="F6" s="6"/>
       <c r="G6" s="7"/>
     </row>
-    <row r="7" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="5"/>
       <c r="B7" s="6"/>
       <c r="C7" s="21" t="s">
@@ -2962,7 +3543,7 @@
       <c r="F7" s="6"/>
       <c r="G7" s="7"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="5"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
@@ -2971,7 +3552,7 @@
       <c r="F8" s="6"/>
       <c r="G8" s="7"/>
     </row>
-    <row r="9" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="5"/>
       <c r="B9" s="6"/>
       <c r="C9" s="21" t="s">
@@ -2984,7 +3565,7 @@
       <c r="F9" s="6"/>
       <c r="G9" s="7"/>
     </row>
-    <row r="10" spans="1:8" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="42" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="5"/>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
@@ -2992,7 +3573,7 @@
       <c r="F10" s="6"/>
       <c r="G10" s="7"/>
     </row>
-    <row r="11" spans="1:8" ht="27.75" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:8" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="5"/>
       <c r="B11" s="6"/>
       <c r="C11" s="20" t="s">
@@ -3008,7 +3589,7 @@
       <c r="F11" s="6"/>
       <c r="G11" s="7"/>
     </row>
-    <row r="12" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A12" s="5"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
@@ -3022,7 +3603,7 @@
       <c r="F12" s="6"/>
       <c r="G12" s="7"/>
     </row>
-    <row r="13" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A13" s="5"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -3036,7 +3617,7 @@
       <c r="F13" s="6"/>
       <c r="G13" s="7"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="5"/>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
@@ -3045,85 +3626,85 @@
       <c r="F14" s="6"/>
       <c r="G14" s="7"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="64" t="s">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A15" s="67" t="s">
         <v>40</v>
       </c>
-      <c r="B15" s="64"/>
-      <c r="C15" s="64"/>
-      <c r="D15" s="64"/>
-      <c r="E15" s="64"/>
-      <c r="F15" s="64"/>
-      <c r="G15" s="65"/>
+      <c r="B15" s="67"/>
+      <c r="C15" s="67"/>
+      <c r="D15" s="67"/>
+      <c r="E15" s="67"/>
+      <c r="F15" s="67"/>
+      <c r="G15" s="68"/>
       <c r="H15" s="5"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="64"/>
-      <c r="B16" s="64"/>
-      <c r="C16" s="64"/>
-      <c r="D16" s="64"/>
-      <c r="E16" s="64"/>
-      <c r="F16" s="64"/>
-      <c r="G16" s="65"/>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A16" s="67"/>
+      <c r="B16" s="67"/>
+      <c r="C16" s="67"/>
+      <c r="D16" s="67"/>
+      <c r="E16" s="67"/>
+      <c r="F16" s="67"/>
+      <c r="G16" s="68"/>
       <c r="H16" s="5"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="H17" s="6"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="66" t="s">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A18" s="69" t="s">
         <v>39</v>
       </c>
-      <c r="B18" s="66"/>
-      <c r="C18" s="66"/>
-      <c r="D18" s="66"/>
-      <c r="E18" s="66"/>
-      <c r="F18" s="66"/>
-      <c r="G18" s="66"/>
+      <c r="B18" s="69"/>
+      <c r="C18" s="69"/>
+      <c r="D18" s="69"/>
+      <c r="E18" s="69"/>
+      <c r="F18" s="69"/>
+      <c r="G18" s="69"/>
       <c r="H18" s="6"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="66"/>
-      <c r="B19" s="66"/>
-      <c r="C19" s="66"/>
-      <c r="D19" s="66"/>
-      <c r="E19" s="66"/>
-      <c r="F19" s="66"/>
-      <c r="G19" s="66"/>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A19" s="69"/>
+      <c r="B19" s="69"/>
+      <c r="C19" s="69"/>
+      <c r="D19" s="69"/>
+      <c r="E19" s="69"/>
+      <c r="F19" s="69"/>
+      <c r="G19" s="69"/>
       <c r="H19" s="6"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="66"/>
-      <c r="B20" s="66"/>
-      <c r="C20" s="66"/>
-      <c r="D20" s="66"/>
-      <c r="E20" s="66"/>
-      <c r="F20" s="66"/>
-      <c r="G20" s="66"/>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A20" s="69"/>
+      <c r="B20" s="69"/>
+      <c r="C20" s="69"/>
+      <c r="D20" s="69"/>
+      <c r="E20" s="69"/>
+      <c r="F20" s="69"/>
+      <c r="G20" s="69"/>
       <c r="H20" s="6"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="66"/>
-      <c r="B21" s="66"/>
-      <c r="C21" s="66"/>
-      <c r="D21" s="66"/>
-      <c r="E21" s="66"/>
-      <c r="F21" s="66"/>
-      <c r="G21" s="66"/>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A21" s="69"/>
+      <c r="B21" s="69"/>
+      <c r="C21" s="69"/>
+      <c r="D21" s="69"/>
+      <c r="E21" s="69"/>
+      <c r="F21" s="69"/>
+      <c r="G21" s="69"/>
       <c r="H21" s="6"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="68" t="s">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A22" s="71" t="s">
         <v>38</v>
       </c>
-      <c r="B22" s="68"/>
-      <c r="C22" s="68"/>
-      <c r="D22" s="68"/>
-      <c r="E22" s="68"/>
-      <c r="F22" s="68"/>
-      <c r="G22" s="68"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B22" s="71"/>
+      <c r="C22" s="71"/>
+      <c r="D22" s="71"/>
+      <c r="E22" s="71"/>
+      <c r="F22" s="71"/>
+      <c r="G22" s="71"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" s="5"/>
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
@@ -3132,18 +3713,18 @@
       <c r="F23" s="6"/>
       <c r="G23" s="7"/>
     </row>
-    <row r="24" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="5"/>
-      <c r="B24" s="69" t="s">
+      <c r="B24" s="72" t="s">
         <v>41</v>
       </c>
-      <c r="C24" s="69"/>
-      <c r="D24" s="69"/>
-      <c r="E24" s="69"/>
+      <c r="C24" s="72"/>
+      <c r="D24" s="72"/>
+      <c r="E24" s="72"/>
       <c r="F24" s="6"/>
       <c r="G24" s="7"/>
     </row>
-    <row r="25" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" s="5"/>
       <c r="B25" s="23" t="s">
         <v>4</v>
@@ -3158,9 +3739,9 @@
         <v>24</v>
       </c>
       <c r="F25" s="6"/>
-      <c r="G25" s="67"/>
-    </row>
-    <row r="26" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G25" s="70"/>
+    </row>
+    <row r="26" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="5"/>
       <c r="B26" s="24">
         <v>0</v>
@@ -3176,9 +3757,9 @@
         <v>0</v>
       </c>
       <c r="F26" s="6"/>
-      <c r="G26" s="67"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G26" s="70"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" s="5"/>
       <c r="B27" s="24">
         <v>50</v>
@@ -3194,9 +3775,9 @@
         <v>3.8</v>
       </c>
       <c r="F27" s="6"/>
-      <c r="G27" s="67"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G27" s="70"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" s="5"/>
       <c r="B28" s="24">
         <v>100</v>
@@ -3212,9 +3793,9 @@
         <v>1.9</v>
       </c>
       <c r="F28" s="6"/>
-      <c r="G28" s="67"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G28" s="70"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" s="5"/>
       <c r="B29" s="24">
         <v>60</v>
@@ -3230,9 +3811,9 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="F29" s="6"/>
-      <c r="G29" s="67"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G29" s="70"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" s="5"/>
       <c r="B30" s="24">
         <v>300</v>
@@ -3248,9 +3829,9 @@
         <v>1.7999999999999998</v>
       </c>
       <c r="F30" s="6"/>
-      <c r="G30" s="67"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G30" s="70"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" s="5"/>
       <c r="B31" s="24">
         <v>350</v>
@@ -3266,9 +3847,9 @@
         <v>0.89999999999999991</v>
       </c>
       <c r="F31" s="6"/>
-      <c r="G31" s="67"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G31" s="70"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" s="5"/>
       <c r="B32" s="24">
         <v>600</v>
@@ -3284,9 +3865,9 @@
         <v>0.5</v>
       </c>
       <c r="F32" s="6"/>
-      <c r="G32" s="67"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G32" s="70"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A33" s="5"/>
       <c r="B33" s="27"/>
       <c r="C33" s="27"/>
@@ -3298,7 +3879,7 @@
       <c r="F33" s="6"/>
       <c r="G33" s="17"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A34" s="5"/>
       <c r="B34" s="6"/>
       <c r="C34" s="6"/>
@@ -3307,7 +3888,7 @@
       <c r="F34" s="6"/>
       <c r="G34" s="7"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A35" s="5"/>
       <c r="B35" s="6"/>
       <c r="C35" s="6"/>
@@ -3316,7 +3897,7 @@
       <c r="F35" s="6"/>
       <c r="G35" s="7"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A36" s="5"/>
       <c r="B36" s="6"/>
       <c r="C36" s="6"/>
@@ -3325,7 +3906,7 @@
       <c r="F36" s="6"/>
       <c r="G36" s="7"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A37" s="15"/>
       <c r="B37" s="15"/>
       <c r="C37" s="15"/>
@@ -3334,7 +3915,7 @@
       <c r="F37" s="15"/>
       <c r="G37" s="15"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A38" s="15"/>
       <c r="B38" s="15"/>
       <c r="C38" s="15"/>
@@ -3343,7 +3924,7 @@
       <c r="F38" s="15"/>
       <c r="G38" s="15"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A39" s="16"/>
       <c r="B39" s="16"/>
       <c r="C39" s="16"/>
@@ -3376,53 +3957,53 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="14.5" zeroHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" customWidth="1"/>
-    <col min="2" max="2" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="11.453125" customWidth="1"/>
+    <col min="2" max="2" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.1796875" customWidth="1"/>
     <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="11.42578125" customWidth="1"/>
-    <col min="10" max="16384" width="11.42578125" hidden="1"/>
+    <col min="8" max="9" width="11.453125" customWidth="1"/>
+    <col min="10" max="16384" width="11.453125" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="3" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="63"/>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
-      <c r="I1" s="63"/>
-    </row>
-    <row r="2" spans="1:9" s="3" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="63"/>
-      <c r="B2" s="63"/>
-      <c r="C2" s="63"/>
-      <c r="D2" s="63"/>
-      <c r="E2" s="63"/>
-      <c r="F2" s="63"/>
-      <c r="G2" s="63"/>
-      <c r="H2" s="63"/>
-      <c r="I2" s="63"/>
-    </row>
-    <row r="3" spans="1:9" s="3" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="63"/>
-      <c r="B3" s="63"/>
-      <c r="C3" s="63"/>
-      <c r="D3" s="63"/>
-      <c r="E3" s="63"/>
-      <c r="F3" s="63"/>
-      <c r="G3" s="63"/>
-      <c r="H3" s="63"/>
-      <c r="I3" s="63"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="3" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="66"/>
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
+      <c r="H1" s="66"/>
+      <c r="I1" s="66"/>
+    </row>
+    <row r="2" spans="1:9" s="3" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="66"/>
+      <c r="B2" s="66"/>
+      <c r="C2" s="66"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="66"/>
+      <c r="H2" s="66"/>
+      <c r="I2" s="66"/>
+    </row>
+    <row r="3" spans="1:9" s="3" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="66"/>
+      <c r="B3" s="66"/>
+      <c r="C3" s="66"/>
+      <c r="D3" s="66"/>
+      <c r="E3" s="66"/>
+      <c r="F3" s="66"/>
+      <c r="G3" s="66"/>
+      <c r="H3" s="66"/>
+      <c r="I3" s="66"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="5"/>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
@@ -3433,7 +4014,7 @@
       <c r="H4" s="6"/>
       <c r="I4" s="12"/>
     </row>
-    <row r="5" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="5"/>
       <c r="B5" s="6"/>
       <c r="C5" s="21" t="s">
@@ -3454,7 +4035,7 @@
       <c r="H5" s="6"/>
       <c r="I5" s="7"/>
     </row>
-    <row r="6" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="5"/>
       <c r="B6" s="6"/>
       <c r="C6" s="34"/>
@@ -3465,7 +4046,7 @@
       <c r="H6" s="6"/>
       <c r="I6" s="7"/>
     </row>
-    <row r="7" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="5"/>
       <c r="B7" s="6"/>
       <c r="C7" s="21" t="s">
@@ -3482,7 +4063,7 @@
       <c r="H7" s="6"/>
       <c r="I7" s="7"/>
     </row>
-    <row r="8" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="5"/>
       <c r="B8" s="6"/>
       <c r="C8" s="35"/>
@@ -3493,7 +4074,7 @@
       <c r="H8" s="6"/>
       <c r="I8" s="7"/>
     </row>
-    <row r="9" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" ht="21" x14ac:dyDescent="0.5">
       <c r="A9" s="5"/>
       <c r="B9" s="6"/>
       <c r="C9" s="43" t="s">
@@ -3509,7 +4090,7 @@
       <c r="H9" s="6"/>
       <c r="I9" s="7"/>
     </row>
-    <row r="10" spans="1:9" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="5"/>
       <c r="B10" s="6"/>
       <c r="C10" s="46" t="s">
@@ -3527,7 +4108,7 @@
       <c r="H10" s="6"/>
       <c r="I10" s="7"/>
     </row>
-    <row r="11" spans="1:9" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="5"/>
       <c r="B11" s="6"/>
       <c r="C11" s="45" t="s">
@@ -3545,7 +4126,7 @@
       <c r="H11" s="6"/>
       <c r="I11" s="7"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="5"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
@@ -3556,121 +4137,121 @@
       <c r="H12" s="6"/>
       <c r="I12" s="7"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="64" t="s">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A13" s="67" t="s">
         <v>40</v>
       </c>
-      <c r="B13" s="64"/>
-      <c r="C13" s="64"/>
-      <c r="D13" s="64"/>
-      <c r="E13" s="64"/>
-      <c r="F13" s="64"/>
-      <c r="G13" s="64"/>
-      <c r="H13" s="64"/>
-      <c r="I13" s="65"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="64"/>
-      <c r="B14" s="64"/>
-      <c r="C14" s="64"/>
-      <c r="D14" s="64"/>
-      <c r="E14" s="64"/>
-      <c r="F14" s="64"/>
-      <c r="G14" s="64"/>
-      <c r="H14" s="64"/>
-      <c r="I14" s="65"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="66" t="s">
+      <c r="B13" s="67"/>
+      <c r="C13" s="67"/>
+      <c r="D13" s="67"/>
+      <c r="E13" s="67"/>
+      <c r="F13" s="67"/>
+      <c r="G13" s="67"/>
+      <c r="H13" s="67"/>
+      <c r="I13" s="68"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A14" s="67"/>
+      <c r="B14" s="67"/>
+      <c r="C14" s="67"/>
+      <c r="D14" s="67"/>
+      <c r="E14" s="67"/>
+      <c r="F14" s="67"/>
+      <c r="G14" s="67"/>
+      <c r="H14" s="67"/>
+      <c r="I14" s="68"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A15" s="69" t="s">
         <v>39</v>
       </c>
-      <c r="B15" s="66"/>
-      <c r="C15" s="66"/>
-      <c r="D15" s="66"/>
-      <c r="E15" s="66"/>
-      <c r="F15" s="66"/>
-      <c r="G15" s="66"/>
-      <c r="H15" s="66"/>
-      <c r="I15" s="66"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="66"/>
-      <c r="B16" s="66"/>
-      <c r="C16" s="66"/>
-      <c r="D16" s="66"/>
-      <c r="E16" s="66"/>
-      <c r="F16" s="66"/>
-      <c r="G16" s="66"/>
-      <c r="H16" s="66"/>
-      <c r="I16" s="66"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="66"/>
-      <c r="B17" s="66"/>
-      <c r="C17" s="66"/>
-      <c r="D17" s="66"/>
-      <c r="E17" s="66"/>
-      <c r="F17" s="66"/>
-      <c r="G17" s="66"/>
-      <c r="H17" s="66"/>
-      <c r="I17" s="66"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="66"/>
-      <c r="B18" s="66"/>
-      <c r="C18" s="66"/>
-      <c r="D18" s="66"/>
-      <c r="E18" s="66"/>
-      <c r="F18" s="66"/>
-      <c r="G18" s="66"/>
-      <c r="H18" s="66"/>
-      <c r="I18" s="66"/>
-    </row>
-    <row r="19" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="70" t="s">
+      <c r="B15" s="69"/>
+      <c r="C15" s="69"/>
+      <c r="D15" s="69"/>
+      <c r="E15" s="69"/>
+      <c r="F15" s="69"/>
+      <c r="G15" s="69"/>
+      <c r="H15" s="69"/>
+      <c r="I15" s="69"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A16" s="69"/>
+      <c r="B16" s="69"/>
+      <c r="C16" s="69"/>
+      <c r="D16" s="69"/>
+      <c r="E16" s="69"/>
+      <c r="F16" s="69"/>
+      <c r="G16" s="69"/>
+      <c r="H16" s="69"/>
+      <c r="I16" s="69"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A17" s="69"/>
+      <c r="B17" s="69"/>
+      <c r="C17" s="69"/>
+      <c r="D17" s="69"/>
+      <c r="E17" s="69"/>
+      <c r="F17" s="69"/>
+      <c r="G17" s="69"/>
+      <c r="H17" s="69"/>
+      <c r="I17" s="69"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A18" s="69"/>
+      <c r="B18" s="69"/>
+      <c r="C18" s="69"/>
+      <c r="D18" s="69"/>
+      <c r="E18" s="69"/>
+      <c r="F18" s="69"/>
+      <c r="G18" s="69"/>
+      <c r="H18" s="69"/>
+      <c r="I18" s="69"/>
+    </row>
+    <row r="19" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="73" t="s">
         <v>38</v>
       </c>
-      <c r="B19" s="71"/>
-      <c r="C19" s="71"/>
-      <c r="D19" s="71"/>
-      <c r="E19" s="71"/>
-      <c r="F19" s="71"/>
-      <c r="G19" s="71"/>
-      <c r="H19" s="71"/>
-      <c r="I19" s="71"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="71"/>
-      <c r="B20" s="71"/>
-      <c r="C20" s="71"/>
-      <c r="D20" s="71"/>
-      <c r="E20" s="71"/>
-      <c r="F20" s="71"/>
-      <c r="G20" s="71"/>
-      <c r="H20" s="71"/>
-      <c r="I20" s="71"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="71"/>
-      <c r="B21" s="71"/>
-      <c r="C21" s="71"/>
-      <c r="D21" s="71"/>
-      <c r="E21" s="71"/>
-      <c r="F21" s="71"/>
-      <c r="G21" s="71"/>
-      <c r="H21" s="71"/>
-      <c r="I21" s="71"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="71"/>
-      <c r="B22" s="71"/>
-      <c r="C22" s="71"/>
-      <c r="D22" s="71"/>
-      <c r="E22" s="71"/>
-      <c r="F22" s="71"/>
-      <c r="G22" s="71"/>
-      <c r="H22" s="71"/>
-      <c r="I22" s="71"/>
+      <c r="B19" s="74"/>
+      <c r="C19" s="74"/>
+      <c r="D19" s="74"/>
+      <c r="E19" s="74"/>
+      <c r="F19" s="74"/>
+      <c r="G19" s="74"/>
+      <c r="H19" s="74"/>
+      <c r="I19" s="74"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A20" s="74"/>
+      <c r="B20" s="74"/>
+      <c r="C20" s="74"/>
+      <c r="D20" s="74"/>
+      <c r="E20" s="74"/>
+      <c r="F20" s="74"/>
+      <c r="G20" s="74"/>
+      <c r="H20" s="74"/>
+      <c r="I20" s="74"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A21" s="74"/>
+      <c r="B21" s="74"/>
+      <c r="C21" s="74"/>
+      <c r="D21" s="74"/>
+      <c r="E21" s="74"/>
+      <c r="F21" s="74"/>
+      <c r="G21" s="74"/>
+      <c r="H21" s="74"/>
+      <c r="I21" s="74"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A22" s="74"/>
+      <c r="B22" s="74"/>
+      <c r="C22" s="74"/>
+      <c r="D22" s="74"/>
+      <c r="E22" s="74"/>
+      <c r="F22" s="74"/>
+      <c r="G22" s="74"/>
+      <c r="H22" s="74"/>
+      <c r="I22" s="74"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -3692,63 +4273,63 @@
       <selection activeCell="A14" sqref="A14:K18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="14.5" zeroHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="5" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="21.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="10" width="11.42578125" style="6" customWidth="1"/>
-    <col min="11" max="11" width="11.42578125" style="7" customWidth="1"/>
-    <col min="12" max="16384" width="11.42578125" hidden="1"/>
+    <col min="1" max="1" width="11.453125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="11.453125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="21.1796875" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.81640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.453125" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="10" width="11.453125" style="6" customWidth="1"/>
+    <col min="11" max="11" width="11.453125" style="7" customWidth="1"/>
+    <col min="12" max="16384" width="11.453125" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="72"/>
-      <c r="B1" s="73"/>
-      <c r="C1" s="73"/>
-      <c r="D1" s="73"/>
-      <c r="E1" s="73"/>
-      <c r="F1" s="73"/>
-      <c r="G1" s="73"/>
-      <c r="H1" s="73"/>
-      <c r="I1" s="73"/>
-      <c r="J1" s="73"/>
-      <c r="K1" s="74"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="75"/>
-      <c r="B2" s="76"/>
-      <c r="C2" s="76"/>
-      <c r="D2" s="76"/>
-      <c r="E2" s="76"/>
-      <c r="F2" s="76"/>
-      <c r="G2" s="76"/>
-      <c r="H2" s="76"/>
-      <c r="I2" s="76"/>
-      <c r="J2" s="76"/>
-      <c r="K2" s="77"/>
-    </row>
-    <row r="3" spans="1:11" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="78"/>
-      <c r="B3" s="79"/>
-      <c r="C3" s="79"/>
-      <c r="D3" s="79"/>
-      <c r="E3" s="79"/>
-      <c r="F3" s="79"/>
-      <c r="G3" s="79"/>
-      <c r="H3" s="79"/>
-      <c r="I3" s="79"/>
-      <c r="J3" s="79"/>
-      <c r="K3" s="80"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A1" s="75"/>
+      <c r="B1" s="76"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="76"/>
+      <c r="I1" s="76"/>
+      <c r="J1" s="76"/>
+      <c r="K1" s="77"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A2" s="78"/>
+      <c r="B2" s="79"/>
+      <c r="C2" s="79"/>
+      <c r="D2" s="79"/>
+      <c r="E2" s="79"/>
+      <c r="F2" s="79"/>
+      <c r="G2" s="79"/>
+      <c r="H2" s="79"/>
+      <c r="I2" s="79"/>
+      <c r="J2" s="79"/>
+      <c r="K2" s="80"/>
+    </row>
+    <row r="3" spans="1:11" ht="61.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="81"/>
+      <c r="B3" s="82"/>
+      <c r="C3" s="82"/>
+      <c r="D3" s="82"/>
+      <c r="E3" s="82"/>
+      <c r="F3" s="82"/>
+      <c r="G3" s="82"/>
+      <c r="H3" s="82"/>
+      <c r="I3" s="82"/>
+      <c r="J3" s="82"/>
+      <c r="K3" s="83"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="H4"/>
       <c r="I4"/>
       <c r="J4"/>
     </row>
-    <row r="5" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C5" s="21" t="s">
         <v>26</v>
       </c>
@@ -3762,7 +4343,7 @@
       <c r="I5"/>
       <c r="J5"/>
     </row>
-    <row r="6" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C6" s="34"/>
       <c r="D6" s="14"/>
       <c r="E6" s="38"/>
@@ -3770,7 +4351,7 @@
       <c r="I6"/>
       <c r="J6"/>
     </row>
-    <row r="7" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C7" s="21" t="s">
         <v>27</v>
       </c>
@@ -3784,14 +4365,14 @@
       <c r="I7"/>
       <c r="J7"/>
     </row>
-    <row r="8" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C8" s="35"/>
       <c r="E8" s="35"/>
       <c r="H8"/>
       <c r="I8"/>
       <c r="J8"/>
     </row>
-    <row r="9" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C9" s="21" t="s">
         <v>21</v>
       </c>
@@ -3806,7 +4387,7 @@
       <c r="I9"/>
       <c r="J9"/>
     </row>
-    <row r="10" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C10" s="36"/>
       <c r="D10" s="13"/>
       <c r="E10" s="40"/>
@@ -3814,105 +4395,105 @@
       <c r="I10"/>
       <c r="J10"/>
     </row>
-    <row r="11" spans="1:11" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="86.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="H11"/>
       <c r="I11"/>
       <c r="J11"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="83" t="s">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A12" s="86" t="s">
         <v>58</v>
       </c>
-      <c r="B12" s="84"/>
-      <c r="C12" s="84"/>
-      <c r="D12" s="84"/>
-      <c r="E12" s="84"/>
-      <c r="F12" s="84"/>
-      <c r="G12" s="84"/>
-      <c r="H12" s="84"/>
-      <c r="I12" s="84"/>
-      <c r="J12" s="84"/>
-      <c r="K12" s="85"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="86"/>
-      <c r="B13" s="64"/>
-      <c r="C13" s="64"/>
-      <c r="D13" s="64"/>
-      <c r="E13" s="64"/>
-      <c r="F13" s="64"/>
-      <c r="G13" s="64"/>
-      <c r="H13" s="64"/>
-      <c r="I13" s="64"/>
-      <c r="J13" s="64"/>
-      <c r="K13" s="65"/>
-    </row>
-    <row r="14" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="81" t="s">
+      <c r="B12" s="87"/>
+      <c r="C12" s="87"/>
+      <c r="D12" s="87"/>
+      <c r="E12" s="87"/>
+      <c r="F12" s="87"/>
+      <c r="G12" s="87"/>
+      <c r="H12" s="87"/>
+      <c r="I12" s="87"/>
+      <c r="J12" s="87"/>
+      <c r="K12" s="88"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A13" s="89"/>
+      <c r="B13" s="67"/>
+      <c r="C13" s="67"/>
+      <c r="D13" s="67"/>
+      <c r="E13" s="67"/>
+      <c r="F13" s="67"/>
+      <c r="G13" s="67"/>
+      <c r="H13" s="67"/>
+      <c r="I13" s="67"/>
+      <c r="J13" s="67"/>
+      <c r="K13" s="68"/>
+    </row>
+    <row r="14" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="84" t="s">
         <v>42</v>
       </c>
-      <c r="B14" s="66"/>
-      <c r="C14" s="66"/>
-      <c r="D14" s="66"/>
-      <c r="E14" s="66"/>
-      <c r="F14" s="66"/>
-      <c r="G14" s="66"/>
-      <c r="H14" s="66"/>
-      <c r="I14" s="66"/>
-      <c r="J14" s="66"/>
-      <c r="K14" s="82"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="81"/>
-      <c r="B15" s="66"/>
-      <c r="C15" s="66"/>
-      <c r="D15" s="66"/>
-      <c r="E15" s="66"/>
-      <c r="F15" s="66"/>
-      <c r="G15" s="66"/>
-      <c r="H15" s="66"/>
-      <c r="I15" s="66"/>
-      <c r="J15" s="66"/>
-      <c r="K15" s="82"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="81"/>
-      <c r="B16" s="66"/>
-      <c r="C16" s="66"/>
-      <c r="D16" s="66"/>
-      <c r="E16" s="66"/>
-      <c r="F16" s="66"/>
-      <c r="G16" s="66"/>
-      <c r="H16" s="66"/>
-      <c r="I16" s="66"/>
-      <c r="J16" s="66"/>
-      <c r="K16" s="82"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="81"/>
-      <c r="B17" s="66"/>
-      <c r="C17" s="66"/>
-      <c r="D17" s="66"/>
-      <c r="E17" s="66"/>
-      <c r="F17" s="66"/>
-      <c r="G17" s="66"/>
-      <c r="H17" s="66"/>
-      <c r="I17" s="66"/>
-      <c r="J17" s="66"/>
-      <c r="K17" s="82"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="81"/>
-      <c r="B18" s="66"/>
-      <c r="C18" s="66"/>
-      <c r="D18" s="66"/>
-      <c r="E18" s="66"/>
-      <c r="F18" s="66"/>
-      <c r="G18" s="66"/>
-      <c r="H18" s="66"/>
-      <c r="I18" s="66"/>
-      <c r="J18" s="66"/>
-      <c r="K18" s="82"/>
+      <c r="B14" s="69"/>
+      <c r="C14" s="69"/>
+      <c r="D14" s="69"/>
+      <c r="E14" s="69"/>
+      <c r="F14" s="69"/>
+      <c r="G14" s="69"/>
+      <c r="H14" s="69"/>
+      <c r="I14" s="69"/>
+      <c r="J14" s="69"/>
+      <c r="K14" s="85"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A15" s="84"/>
+      <c r="B15" s="69"/>
+      <c r="C15" s="69"/>
+      <c r="D15" s="69"/>
+      <c r="E15" s="69"/>
+      <c r="F15" s="69"/>
+      <c r="G15" s="69"/>
+      <c r="H15" s="69"/>
+      <c r="I15" s="69"/>
+      <c r="J15" s="69"/>
+      <c r="K15" s="85"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A16" s="84"/>
+      <c r="B16" s="69"/>
+      <c r="C16" s="69"/>
+      <c r="D16" s="69"/>
+      <c r="E16" s="69"/>
+      <c r="F16" s="69"/>
+      <c r="G16" s="69"/>
+      <c r="H16" s="69"/>
+      <c r="I16" s="69"/>
+      <c r="J16" s="69"/>
+      <c r="K16" s="85"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A17" s="84"/>
+      <c r="B17" s="69"/>
+      <c r="C17" s="69"/>
+      <c r="D17" s="69"/>
+      <c r="E17" s="69"/>
+      <c r="F17" s="69"/>
+      <c r="G17" s="69"/>
+      <c r="H17" s="69"/>
+      <c r="I17" s="69"/>
+      <c r="J17" s="69"/>
+      <c r="K17" s="85"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A18" s="84"/>
+      <c r="B18" s="69"/>
+      <c r="C18" s="69"/>
+      <c r="D18" s="69"/>
+      <c r="E18" s="69"/>
+      <c r="F18" s="69"/>
+      <c r="G18" s="69"/>
+      <c r="H18" s="69"/>
+      <c r="I18" s="69"/>
+      <c r="J18" s="69"/>
+      <c r="K18" s="85"/>
     </row>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="JNEr92pX3Y356TJzzAmYcRWWL4WENMpzmC40fnNV6AG2IdlrZsuS9ue6A9/jL/HA4AAwxMwZd+KWYBjOGdWalw==" saltValue="aAMA071bt/Ny0MgWzzLp1Q==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
@@ -3936,55 +4517,56 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="14.5" zeroHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="49" customWidth="1"/>
-    <col min="2" max="2" width="26.42578125" style="49" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.7109375" style="49" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.28515625" style="49" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.5703125" style="49" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.5703125" style="49" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="11.42578125" style="49" customWidth="1"/>
-    <col min="10" max="16384" width="11.42578125" style="49" hidden="1"/>
+    <col min="1" max="1" width="11.453125" style="49" customWidth="1"/>
+    <col min="2" max="2" width="32.453125" style="49" customWidth="1"/>
+    <col min="3" max="3" width="32.7265625" style="49" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.26953125" style="49" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.54296875" style="49" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.54296875" style="49" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="41.453125" style="49" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="11.453125" style="49" customWidth="1"/>
+    <col min="10" max="16384" width="11.453125" style="49" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="87"/>
-      <c r="B1" s="88"/>
-      <c r="C1" s="88"/>
-      <c r="D1" s="88"/>
-      <c r="E1" s="88"/>
-      <c r="F1" s="88"/>
-      <c r="G1" s="88"/>
-      <c r="H1" s="88"/>
-      <c r="I1" s="89"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="90"/>
-      <c r="B2" s="63"/>
-      <c r="C2" s="63"/>
-      <c r="D2" s="63"/>
-      <c r="E2" s="63"/>
-      <c r="F2" s="63"/>
-      <c r="G2" s="63"/>
-      <c r="H2" s="63"/>
-      <c r="I2" s="91"/>
-    </row>
-    <row r="3" spans="1:9" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="92"/>
-      <c r="B3" s="93"/>
-      <c r="C3" s="93"/>
-      <c r="D3" s="93"/>
-      <c r="E3" s="93"/>
-      <c r="F3" s="93"/>
-      <c r="G3" s="93"/>
-      <c r="H3" s="93"/>
-      <c r="I3" s="94"/>
-    </row>
-    <row r="4" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1" s="90"/>
+      <c r="B1" s="91"/>
+      <c r="C1" s="91"/>
+      <c r="D1" s="91"/>
+      <c r="E1" s="91"/>
+      <c r="F1" s="91"/>
+      <c r="G1" s="91"/>
+      <c r="H1" s="91"/>
+      <c r="I1" s="92"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" s="93"/>
+      <c r="B2" s="66"/>
+      <c r="C2" s="66"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="66"/>
+      <c r="H2" s="66"/>
+      <c r="I2" s="94"/>
+    </row>
+    <row r="3" spans="1:9" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="95"/>
+      <c r="B3" s="96"/>
+      <c r="C3" s="96"/>
+      <c r="D3" s="96"/>
+      <c r="E3" s="96"/>
+      <c r="F3" s="96"/>
+      <c r="G3" s="96"/>
+      <c r="H3" s="96"/>
+      <c r="I3" s="97"/>
+    </row>
+    <row r="4" spans="1:9" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="53"/>
       <c r="B4" s="54"/>
       <c r="C4" s="54"/>
@@ -3995,18 +4577,20 @@
       <c r="H4" s="54"/>
       <c r="I4" s="55"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="56"/>
       <c r="B5" s="41"/>
       <c r="C5" s="41"/>
       <c r="D5" s="41"/>
       <c r="E5" s="41"/>
       <c r="F5" s="41"/>
-      <c r="G5" s="41"/>
+      <c r="G5" s="99" t="s">
+        <v>61</v>
+      </c>
       <c r="H5" s="41"/>
       <c r="I5" s="57"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="56"/>
       <c r="B6" s="41"/>
       <c r="C6" s="13" t="s">
@@ -4019,34 +4603,38 @@
         <v>59</v>
       </c>
       <c r="F6" s="41"/>
-      <c r="G6" s="41"/>
+      <c r="G6" s="99" t="s">
+        <v>62</v>
+      </c>
       <c r="H6" s="41"/>
       <c r="I6" s="57"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="56"/>
       <c r="B7" s="41"/>
       <c r="C7" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="D7" s="96">
+      <c r="D7" s="64">
         <v>100</v>
       </c>
       <c r="E7" s="51" t="s">
         <v>48</v>
       </c>
       <c r="F7" s="41"/>
-      <c r="G7" s="41"/>
+      <c r="G7" s="99" t="s">
+        <v>63</v>
+      </c>
       <c r="H7" s="41"/>
       <c r="I7" s="57"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="56"/>
       <c r="B8" s="41"/>
       <c r="C8" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="D8" s="95">
+      <c r="D8" s="63">
         <f>D7*30</f>
         <v>3000</v>
       </c>
@@ -4054,11 +4642,13 @@
         <v>49</v>
       </c>
       <c r="F8" s="41"/>
-      <c r="G8" s="41"/>
+      <c r="G8" s="99" t="s">
+        <v>64</v>
+      </c>
       <c r="H8" s="41"/>
       <c r="I8" s="57"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="56"/>
       <c r="B9" s="41"/>
       <c r="C9" s="13" t="s">
@@ -4072,22 +4662,22 @@
         <v>60</v>
       </c>
       <c r="F9" s="41"/>
-      <c r="G9" s="41"/>
+      <c r="G9" s="98"/>
       <c r="H9" s="41"/>
       <c r="I9" s="57"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="56"/>
       <c r="B10" s="41"/>
       <c r="C10" s="50"/>
       <c r="D10" s="41"/>
       <c r="E10" s="51"/>
       <c r="F10" s="41"/>
-      <c r="G10" s="41"/>
+      <c r="G10" s="98"/>
       <c r="H10" s="41"/>
       <c r="I10" s="57"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="56"/>
       <c r="B11" s="41"/>
       <c r="C11" s="50"/>
@@ -4098,11 +4688,13 @@
         <v>52</v>
       </c>
       <c r="F11" s="41"/>
-      <c r="G11" s="41"/>
+      <c r="G11" s="99" t="s">
+        <v>70</v>
+      </c>
       <c r="H11" s="41"/>
       <c r="I11" s="57"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="56"/>
       <c r="B12" s="41"/>
       <c r="C12" s="13" t="s">
@@ -4115,13 +4707,17 @@
         <v>1.2500000000000001E-2</v>
       </c>
       <c r="F12" s="41"/>
-      <c r="G12" s="41"/>
+      <c r="G12" s="99" t="s">
+        <v>69</v>
+      </c>
       <c r="H12" s="41"/>
       <c r="I12" s="57"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="56"/>
-      <c r="B13" s="41"/>
+      <c r="B13" s="99" t="s">
+        <v>65</v>
+      </c>
       <c r="C13" s="13" t="s">
         <v>53</v>
       </c>
@@ -4129,29 +4725,31 @@
         <f>D6*D12</f>
         <v>7000.0000000000009</v>
       </c>
-      <c r="E13" s="97">
+      <c r="E13" s="65">
         <f>D6*E12</f>
         <v>2500</v>
       </c>
       <c r="F13" s="51" t="s">
         <v>37</v>
       </c>
-      <c r="G13" s="41"/>
+      <c r="G13" s="99" t="s">
+        <v>66</v>
+      </c>
       <c r="H13" s="41"/>
       <c r="I13" s="57"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="56"/>
       <c r="B14" s="41"/>
       <c r="C14" s="8"/>
       <c r="D14" s="41"/>
       <c r="E14" s="41"/>
       <c r="F14" s="41"/>
-      <c r="G14" s="41"/>
+      <c r="G14" s="98"/>
       <c r="H14" s="41"/>
       <c r="I14" s="57"/>
     </row>
-    <row r="15" spans="1:9" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:9" ht="26.5" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A15" s="56"/>
       <c r="B15" s="41"/>
       <c r="C15" s="13" t="s">
@@ -4165,11 +4763,13 @@
         <v>56</v>
       </c>
       <c r="F15" s="41"/>
-      <c r="G15" s="41"/>
+      <c r="G15" s="99" t="s">
+        <v>67</v>
+      </c>
       <c r="H15" s="41"/>
       <c r="I15" s="57"/>
     </row>
-    <row r="16" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="56"/>
       <c r="B16" s="41"/>
       <c r="C16" s="13" t="s">
@@ -4181,11 +4781,13 @@
       </c>
       <c r="E16" s="41"/>
       <c r="F16" s="41"/>
-      <c r="G16" s="41"/>
+      <c r="G16" s="99" t="s">
+        <v>68</v>
+      </c>
       <c r="H16" s="41"/>
       <c r="I16" s="57"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="56"/>
       <c r="B17" s="41"/>
       <c r="C17" s="41"/>
@@ -4196,18 +4798,18 @@
       <c r="H17" s="41"/>
       <c r="I17" s="57"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="63" t="s">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A18" s="66" t="s">
         <v>57</v>
       </c>
-      <c r="B18" s="63"/>
-      <c r="C18" s="63"/>
-      <c r="D18" s="63"/>
-      <c r="E18" s="63"/>
-      <c r="F18" s="63"/>
-      <c r="G18" s="63"/>
-      <c r="H18" s="63"/>
-      <c r="I18" s="63"/>
+      <c r="B18" s="66"/>
+      <c r="C18" s="66"/>
+      <c r="D18" s="66"/>
+      <c r="E18" s="66"/>
+      <c r="F18" s="66"/>
+      <c r="G18" s="66"/>
+      <c r="H18" s="66"/>
+      <c r="I18" s="66"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -4227,9 +4829,9 @@
       <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1">
         <v>1</v>
       </c>
@@ -4238,7 +4840,7 @@
         <v>210000</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>4</v>
       </c>
@@ -4247,7 +4849,7 @@
         <v>5460</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>6</v>
       </c>
@@ -4256,7 +4858,7 @@
         <v>10080</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>12</v>
       </c>
@@ -4265,7 +4867,7 @@
         <v>25200</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>24</v>
       </c>
@@ -4274,7 +4876,7 @@
         <v>63000</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>36</v>
       </c>
@@ -4296,9 +4898,9 @@
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -4312,7 +4914,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -4326,7 +4928,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -4340,7 +4942,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -4354,7 +4956,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -4368,7 +4970,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -4382,7 +4984,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -4396,7 +4998,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
@@ -4422,15 +5024,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D9FD89AD9B50DB49A7A335C5DE569E32" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="892c7a54193b534b1a830f214a0a1efd">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7215713de735d43f81e1c38e5e111042">
     <xsd:element name="properties">
@@ -4544,6 +5137,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EED13452-51A6-428E-A6C4-6903872C3093}">
   <ds:schemaRefs>
@@ -4560,14 +5162,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3DCF46F-0408-47BC-8606-5F9EE72C4C5F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A19BCDAB-246D-4321-AF5D-DE1C3733986A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4581,4 +5175,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3DCF46F-0408-47BC-8606-5F9EE72C4C5F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>